<commit_message>
update publication list with valid dates
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6ED1AD7-25E7-419B-A886-06FDFCAFB675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2104F443-096D-43D2-8349-910CD8BCCDE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="330">
   <si>
     <t>pub_date</t>
   </si>
@@ -369,9 +369,6 @@
     <t>European Journal of Physiotherapy</t>
   </si>
   <si>
-    <t>Lim, W.S., Sharma, S., Devan, H. (2020).Physiotherapists’ attitudes towards and challenges of working in a referral-based practice setting–a systematic scoping review. European Journal of Physiotherapy,</t>
-  </si>
-  <si>
     <t>Assessing implementation readiness and success of an e-resource to improve prelicensure physical therapy workforce capacity to manage rheumatoid arthritis</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>Bannuru RR, Osani MC, Vaysbrot EE, et al. OARSI guidelines for the non-surgical management of knee, hip, and polyarticular osteoarthritis. Osteoarthritis and Cartilage 2019;27(11):1578-1589.</t>
   </si>
   <si>
-    <t>2019-11</t>
-  </si>
-  <si>
     <t>Bennell KL, Nelligan R, Dobson F, et al. Effectiveness of an internet-delivered exercise and pain-coping skills training intervention for persons with chronic knee pain: A randomized trial. Annals of Internal Medicine 2017;166(7):453-462.</t>
   </si>
   <si>
@@ -597,15 +591,9 @@
     <t>Skou ST, Pedersen BK, Abbott JH, et al. Physical activity and exercise therapy benefit more than just symptoms and impairments in people with hip and knee osteoarthritis. Journal of Orthopaedic and Sports Physical Therapy 2018;48(6):439-447.</t>
   </si>
   <si>
-    <t>2018-06</t>
-  </si>
-  <si>
     <t>Briggs AM, Jordan JE, Jennings M, et al. Supporting the Evaluation and Implementation of Musculoskeletal Models of Care: A Globally Informed Framework for Judging Readiness and Success. Arthritis Care and Research 2017;69(4):567-577.</t>
   </si>
   <si>
-    <t>2017-04</t>
-  </si>
-  <si>
     <t>Sharma S, Palanchoke J, Reed D, et al. Translation, cross-cultural adaptation and psychometric properties of the Nepali versions of numerical pain rating scale and global rating of change. Health and Quality of Life Outcomes 2017;15:236.</t>
   </si>
   <si>
@@ -633,9 +621,6 @@
     <t>Pathak A, Sharma S, Jensen MP. The utility and validity of pain intensity rating scales for use in developing countries. Pain Reports 2018;3(5):e672.</t>
   </si>
   <si>
-    <t>2018-09</t>
-  </si>
-  <si>
     <t>Bennell KL, Nelligan RK, Rini C, et al. Effects of internet-based pain coping skills training before home exercise for individuals with hip osteoarthritis (HOPE trial): A randomised controlled trial. Pain 2018;159(9):1833-1842.</t>
   </si>
   <si>
@@ -654,33 +639,12 @@
     <t>Wilson R, Abbott JH. Age, period and cohort effects on body mass index in New Zealand, 1997–2038. Australian and New Zealand Journal of Public Health 2018;42(4):396-402.</t>
   </si>
   <si>
-    <t>2018-08</t>
-  </si>
-  <si>
     <t>Abbott JH, Wilson R, Pinto D, et al. Incremental clinical effectiveness and cost effectiveness of providing supervised physiotherapy in addition to usual medical care in patients with osteoarthritis of the hip or knee: 2-year results of the MOA randomised controlled trial. Osteoarthritis and Cartilage 2019;27(3):424-434.</t>
   </si>
   <si>
-    <t>2019-03</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
     <t>Gwynne-Jones DP, Hutton LR, Stout KM, et al. The Joint Clinic: Managing Excess Demand for Hip and Knee Osteoarthritis Referrals Using a New Physiotherapy-Led Outpatient Service. Journal of Arthroplasty 2018;33(4):983-987.</t>
   </si>
   <si>
-    <t>2018-04</t>
-  </si>
-  <si>
     <t>joint-clinic</t>
   </si>
   <si>
@@ -696,9 +660,6 @@
     <t>exercise-manual-therapy-booster-sessions-knee-oa</t>
   </si>
   <si>
-    <t>2018-01</t>
-  </si>
-  <si>
     <t>KC S, Sharma S, Ginn K, et al. Cross-cultural adaptation and measurement properties of the Nepali version of the DASH (disability of arm, shoulder and hand) in patients with shoulder pain. Health and Quality of Life Outcomes 2019;17:51.</t>
   </si>
   <si>
@@ -738,9 +699,6 @@
     <t>Sharma S, Ferreira-Valente A, Williams ACdC, et al. Group differences between countries and between languages in pain-related beliefs, coping, and catastrophizing in chronic pain: A systematic review. Pain Medicine 2020;21(9):1847-1862.</t>
   </si>
   <si>
-    <t>2020-09</t>
-  </si>
-  <si>
     <t>properties-nepali-pain-catastrophizing-scale</t>
   </si>
   <si>
@@ -789,9 +747,6 @@
     <t>delivering-right-care-lbp-nepal</t>
   </si>
   <si>
-    <t>2019-06</t>
-  </si>
-  <si>
     <t>free-rct</t>
   </si>
   <si>
@@ -810,15 +765,9 @@
     <t>health-system-strengthening-pain</t>
   </si>
   <si>
-    <t>2019-12</t>
-  </si>
-  <si>
     <t>Abbott JH, Hobbs C, Gwynne-Jones D. The ShortMAC: Minimum Important Change of a Reduced Version of the Western Ontario and McMaster Universities Osteoarthritis Index. Journal of Orthopaedic and Sports Physical Therapy 2018;48(2):81-86.</t>
   </si>
   <si>
-    <t>2018-02</t>
-  </si>
-  <si>
     <t>elf-cluster-rct-protocol</t>
   </si>
   <si>
@@ -897,9 +846,6 @@
     <t>Gwynne-Jones JH, Wilson RA, Wong JMY, et al. The Outcomes of Nonoperative Management of Patients With Hip and Knee Osteoarthritis Triaged to a Physiotherapy-Led Clinic at Minimum 5-Year Follow-Up and Factors Associated With Progression to Surgery. Journal of Arthroplasty 2020;35(6):1497-1503.</t>
   </si>
   <si>
-    <t>2020-06</t>
-  </si>
-  <si>
     <t>digital-technologies-self-management-pain</t>
   </si>
   <si>
@@ -933,9 +879,6 @@
     <t>risk-factors-chronic-opioid-use</t>
   </si>
   <si>
-    <t>2020-11</t>
-  </si>
-  <si>
     <t>development-nzmoa-model</t>
   </si>
   <si>
@@ -984,9 +927,6 @@
     <t>Ribeiro DC, Milosavljevic S, Terry J, Abbott JH. Effectiveness of a lumbopelvic monitor and feedback device to change postural behaviour: The ELF cluster randomised controlled trial. Occupational and Environmental Medicine 2020;77(7):462-469.</t>
   </si>
   <si>
-    <t>2020-07</t>
-  </si>
-  <si>
     <t>prioritisation-tool-first-specialist-appointment</t>
   </si>
   <si>
@@ -994,6 +934,87 @@
   </si>
   <si>
     <t>Ribeiro DC, Macznik AK, Milosavljevic S, Abbott JH. Effectiveness of extrinsic feedback for management of non-specific low back pain: A systematic review protocol. BMJ Open 2018;8:e021259.</t>
+  </si>
+  <si>
+    <t>2019-11-01</t>
+  </si>
+  <si>
+    <t>2018-06-01</t>
+  </si>
+  <si>
+    <t>2017-04-01</t>
+  </si>
+  <si>
+    <t>2018-09-01</t>
+  </si>
+  <si>
+    <t>2018-08-01</t>
+  </si>
+  <si>
+    <t>2019-03-01</t>
+  </si>
+  <si>
+    <t>2018-04-01</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2019-09-18</t>
+  </si>
+  <si>
+    <t>2019-06-01</t>
+  </si>
+  <si>
+    <t>2019-12-01</t>
+  </si>
+  <si>
+    <t>2018-02-01</t>
+  </si>
+  <si>
+    <t>2020-06-01</t>
+  </si>
+  <si>
+    <t>2020-11-01</t>
+  </si>
+  <si>
+    <t>2020-07-01</t>
+  </si>
+  <si>
+    <t>2020-02-18</t>
+  </si>
+  <si>
+    <t>2019-09-09</t>
+  </si>
+  <si>
+    <t>2019-08-30</t>
+  </si>
+  <si>
+    <t>2017-10-01</t>
+  </si>
+  <si>
+    <t>2020-04-01</t>
+  </si>
+  <si>
+    <t>2017-10-17</t>
+  </si>
+  <si>
+    <t>2020-10-01</t>
+  </si>
+  <si>
+    <t>2019-05-19</t>
+  </si>
+  <si>
+    <t>2020-08-17</t>
+  </si>
+  <si>
+    <t>Lim, W.S., Sharma, S., Devan, H. (2020).Physiotherapists’ attitudes towards and challenges of working in a referral-based practice setting–a systematic scoping review. European Journal of Physiotherapy, In Press.</t>
+  </si>
+  <si>
+    <t>2020-03-24</t>
+  </si>
+  <si>
+    <t>2017-09-01</t>
   </si>
 </sst>
 </file>
@@ -1195,10 +1216,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1533,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1572,8 +1594,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>186</v>
+      <c r="A2" s="3" t="s">
+        <v>303</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1583,18 +1605,18 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>188</v>
+      <c r="A3" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -1604,18 +1626,18 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>190</v>
+      <c r="A4" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -1625,18 +1647,18 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>192</v>
+      <c r="A5" s="3" t="s">
+        <v>305</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -1646,18 +1668,18 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -1666,18 +1688,18 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1686,18 +1708,18 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1706,18 +1728,18 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>202</v>
+        <v>306</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -1726,18 +1748,18 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1746,18 +1768,18 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>202</v>
+      <c r="A11" s="3" t="s">
+        <v>306</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
@@ -1767,18 +1789,18 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>209</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -1787,18 +1809,18 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>211</v>
+        <v>308</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1807,18 +1829,18 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F13" t="s">
         <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -1827,18 +1849,18 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="F14" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>209</v>
+        <v>307</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
@@ -1847,18 +1869,18 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F15" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>223</v>
+      <c r="A16" s="3" t="s">
+        <v>310</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>40</v>
@@ -1868,18 +1890,18 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>225</v>
+      <c r="A17" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>42</v>
@@ -1889,18 +1911,18 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>202</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
@@ -1909,18 +1931,18 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F18" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="G18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>231</v>
+      <c r="A19" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>45</v>
@@ -1930,18 +1952,18 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
@@ -1950,38 +1972,38 @@
         <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>237</v>
+        <v>270</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="E21" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="F21" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="G21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
@@ -1990,18 +2012,18 @@
         <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="F22" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>213</v>
+      <c r="A23" s="3" t="s">
+        <v>311</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>51</v>
@@ -2014,15 +2036,15 @@
         <v>53</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -2031,18 +2053,18 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="F24" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>212</v>
+        <v>309</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
@@ -2054,15 +2076,15 @@
         <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="G25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>215</v>
+      <c r="A26" s="3" t="s">
+        <v>318</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>58</v>
@@ -2075,35 +2097,35 @@
         <v>60</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="E27" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="F27" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>202</v>
+        <v>306</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
@@ -2112,18 +2134,18 @@
         <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="F28" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>254</v>
+      <c r="A29" s="3" t="s">
+        <v>312</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>63</v>
@@ -2133,18 +2155,18 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>213</v>
+      <c r="A30" s="3" t="s">
+        <v>319</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>65</v>
@@ -2157,15 +2179,15 @@
         <v>67</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B31" t="s">
         <v>68</v>
@@ -2174,18 +2196,18 @@
         <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F31" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="G31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>261</v>
+        <v>313</v>
       </c>
       <c r="B32" t="s">
         <v>70</v>
@@ -2194,18 +2216,18 @@
         <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F32" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="G32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>263</v>
+        <v>314</v>
       </c>
       <c r="B33" t="s">
         <v>71</v>
@@ -2214,18 +2236,18 @@
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="F33" t="s">
         <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="B34" t="s">
         <v>73</v>
@@ -2234,39 +2256,39 @@
         <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="F34" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="G34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>213</v>
+      <c r="A35" s="3" t="s">
+        <v>313</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>213</v>
+      <c r="A36" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>76</v>
@@ -2279,36 +2301,36 @@
         <v>78</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>214</v>
+      <c r="A37" s="3" t="s">
+        <v>321</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>213</v>
+      <c r="A38" s="3" t="s">
+        <v>308</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>81</v>
@@ -2321,32 +2343,32 @@
         <v>83</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="B39" t="s">
         <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="E39" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="F39" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>186</v>
+        <v>303</v>
       </c>
       <c r="B40" t="s">
         <v>85</v>
@@ -2355,35 +2377,35 @@
         <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="F40" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B41" t="s">
         <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="E41" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="F41" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="B42" t="s">
         <v>87</v>
@@ -2392,18 +2414,18 @@
         <v>88</v>
       </c>
       <c r="E42" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="F42" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="B43" t="s">
         <v>89</v>
@@ -2412,18 +2434,18 @@
         <v>90</v>
       </c>
       <c r="E43" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="F43" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B44" t="s">
         <v>91</v>
@@ -2432,18 +2454,18 @@
         <v>38</v>
       </c>
       <c r="E44" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="F44" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="G44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>215</v>
+      <c r="A45" s="3" t="s">
+        <v>315</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>92</v>
@@ -2456,15 +2478,15 @@
         <v>94</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>215</v>
+      <c r="A46" s="3" t="s">
+        <v>322</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>95</v>
@@ -2477,15 +2499,15 @@
         <v>96</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>237</v>
+        <v>270</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
@@ -2494,18 +2516,18 @@
         <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="F47" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="G47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="B48" t="s">
         <v>98</v>
@@ -2514,18 +2536,18 @@
         <v>50</v>
       </c>
       <c r="E48" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="F48" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="G48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>214</v>
+      <c r="A49" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>99</v>
@@ -2538,15 +2560,15 @@
         <v>101</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>215</v>
+      <c r="A50" s="3" t="s">
+        <v>324</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>102</v>
@@ -2559,15 +2581,15 @@
         <v>104</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B51" t="s">
         <v>105</v>
@@ -2576,18 +2598,18 @@
         <v>38</v>
       </c>
       <c r="E51" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="F51" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="G51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="B52" t="s">
         <v>106</v>
@@ -2596,18 +2618,18 @@
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="F52" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="G52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>213</v>
+      <c r="A53" s="3" t="s">
+        <v>325</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>107</v>
@@ -2620,15 +2642,15 @@
         <v>108</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>215</v>
+      <c r="A54" s="3" t="s">
+        <v>326</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>109</v>
@@ -2641,15 +2663,15 @@
         <v>111</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>215</v>
+      <c r="A55" s="3" t="s">
+        <v>328</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>112</v>
@@ -2659,155 +2681,155 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
         <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="F58" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="G58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
         <v>113</v>
       </c>
       <c r="E59" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="F59" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="G59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" t="s">
         <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="F60" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="G60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
         <v>122</v>
       </c>
-      <c r="C61" t="s">
-        <v>123</v>
-      </c>
       <c r="E61" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="F61" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="G61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>237</v>
+        <v>270</v>
       </c>
       <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
         <v>124</v>
       </c>
-      <c r="C62" t="s">
-        <v>125</v>
-      </c>
       <c r="E62" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="F62" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="G62" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct text formatting error
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E8424-6767-45A6-BECE-8C15E5074B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628F300A-58D0-4DA1-9194-70DAB1BEB184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1002,9 +1002,6 @@
     <t>2021-01-21</t>
   </si>
   <si>
-    <t>Total hip and knee arthroplasty are highly cost-effective procedures: The importance of duration of follow-up</t>
-  </si>
-  <si>
     <t>Wilson RA, Gwynne-Jones DP, Sullivan TA, Abbott JH. Total hip and knee arthroplasty are highly cost-effective procedures: The importance of duration of follow-up. Journal of Arthroplasty 2021;36(6):1864-1872.</t>
   </si>
   <si>
@@ -1081,6 +1078,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1016/j.ocarto.2021.100160</t>
+  </si>
+  <si>
+    <t>Total hip and knee arthroplasty are highly cost-effective procedures: The importance of duration of follow-up</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1622,7 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2113,13 +2113,13 @@
         <v>302</v>
       </c>
       <c r="B24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F24" t="s">
         <v>198</v>
@@ -2618,14 +2618,14 @@
         <v>322</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>283</v>
@@ -2680,14 +2680,14 @@
         <v>310</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>91</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>268</v>
@@ -2903,79 +2903,79 @@
         <v>324</v>
       </c>
       <c r="B63" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="C63" t="s">
         <v>37</v>
       </c>
       <c r="E63" t="s">
+        <v>325</v>
+      </c>
+      <c r="F63" t="s">
         <v>326</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>327</v>
-      </c>
-      <c r="G63" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B64" t="s">
         <v>335</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>336</v>
       </c>
-      <c r="C64" t="s">
+      <c r="E64" t="s">
         <v>337</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>338</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>339</v>
-      </c>
-      <c r="G64" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B65" t="s">
         <v>341</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>336</v>
+      </c>
+      <c r="E65" t="s">
         <v>342</v>
       </c>
-      <c r="C65" t="s">
-        <v>337</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>343</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>344</v>
-      </c>
-      <c r="G65" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B66" t="s">
         <v>346</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>347</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>348</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>349</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>350</v>
-      </c>
-      <c r="G66" t="s">
-        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor updates to publications excel workbook
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628F300A-58D0-4DA1-9194-70DAB1BEB184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{628F300A-58D0-4DA1-9194-70DAB1BEB184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4E004DC-F944-4A41-B6B3-B1713B1B2FCD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
@@ -1282,11 +1282,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="14"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1621,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2084,7 +2085,7 @@
       <c r="F22" t="s">
         <v>26</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="4" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2959,22 +2960,23 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="E66" t="s">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="2" t="s">
         <v>350</v>
       </c>
     </row>
@@ -2983,7 +2985,10 @@
     <sortCondition ref="A2:A62"/>
     <sortCondition ref="E2:E62"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="G22" r:id="rId1" xr:uid="{9871C283-4EA4-4321-BCFE-65A20C93EBB0}"/>
+  </hyperlinks>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>